<commit_message>
Add color to the excel
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bertaruiz/Desktop/BERTA/ESTUDIOS/UNIVERSIDAD/MÁSTER GD/TFM/PAPER/START/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9EAF3-7799-FA4D-8A4B-5D5E8432BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB663E1-C2FC-AF43-BA01-771BA1F94FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="12260" windowHeight="12580" activeTab="4" xr2:uid="{04256E5A-9FC3-4ED9-8234-05D2531DDDEE}"/>
   </bookViews>
@@ -655,7 +655,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1107,7 +1107,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F19"/>
+      <selection sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1163,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1186,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1221,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1241,10 +1241,10 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1333,10 +1333,10 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1347,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1370,10 +1370,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1393,13 +1393,13 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1425,10 +1425,10 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1494,10 +1494,10 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1508,7 +1508,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1537,13 +1537,13 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>

</xml_diff>